<commit_message>
acadia web scraping done
</commit_message>
<xml_diff>
--- a/NSCCITCourses.xlsx
+++ b/NSCCITCourses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassa\Documents\NSCC\CARET\CARETAnalysis-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31CE2054-B26A-46C3-BBC0-A0492D0147AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4225DAB-1BCE-4D3A-B159-E6C1B216D1EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="839" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,13 +22,13 @@
     <sheet name="Data Analytics" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="6" hidden="1">'Data Analytics'!$A$1:$B$63</definedName>
-    <definedName name="ExternalData_2" localSheetId="5" hidden="1">'Database Admin'!$A$1:$B$63</definedName>
-    <definedName name="ExternalData_3" localSheetId="4" hidden="1">'Embedded Systems'!$A$1:$B$33</definedName>
-    <definedName name="ExternalData_4" localSheetId="3" hidden="1">'IT Generalist'!$A$1:$B$59</definedName>
-    <definedName name="ExternalData_5" localSheetId="2" hidden="1">Programming!$A$1:$B$53</definedName>
-    <definedName name="ExternalData_6" localSheetId="1" hidden="1">'Web Programming'!$A$1:$B$53</definedName>
-    <definedName name="ExternalData_7" localSheetId="0" hidden="1">'Systems Management &amp; Security'!$A$1:$B$61</definedName>
+    <definedName name="ExternalData_1" localSheetId="6" hidden="1">'Data Analytics'!$A$1:$B$61</definedName>
+    <definedName name="ExternalData_2" localSheetId="5" hidden="1">'Database Admin'!$A$1:$B$61</definedName>
+    <definedName name="ExternalData_3" localSheetId="4" hidden="1">'Embedded Systems'!$A$1:$B$31</definedName>
+    <definedName name="ExternalData_4" localSheetId="3" hidden="1">'IT Generalist'!$A$1:$B$57</definedName>
+    <definedName name="ExternalData_5" localSheetId="2" hidden="1">Programming!$A$1:$B$51</definedName>
+    <definedName name="ExternalData_6" localSheetId="1" hidden="1">'Web Programming'!$A$1:$B$51</definedName>
+    <definedName name="ExternalData_7" localSheetId="0" hidden="1">'Systems Management &amp; Security'!$A$1:$B$59</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="176">
   <si>
     <t>Course Title</t>
   </si>
@@ -640,6 +640,7 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -702,10 +703,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -714,6 +711,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -807,41 +807,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F2A0DA95-7DF6-4F20-A766-84CD1C095343}" name="NSCCITSysManSec" displayName="NSCCITSysManSec" ref="A1:B61" tableType="queryTable" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:B61" xr:uid="{7CDA9DD1-B254-40A8-889C-C71A0DD60F81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F2A0DA95-7DF6-4F20-A766-84CD1C095343}" name="NSCCITSysManSec" displayName="NSCCITSysManSec" ref="A1:B59" tableType="queryTable" totalsRowShown="0" dataDxfId="20">
+  <autoFilter ref="A1:B59" xr:uid="{7CDA9DD1-B254-40A8-889C-C71A0DD60F81}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E1B31EEF-FEBC-4E73-8E83-57BBAA75208B}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{0923EF4A-D990-4660-B1B6-57E0A5695B3C}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E1B31EEF-FEBC-4E73-8E83-57BBAA75208B}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{0923EF4A-D990-4660-B1B6-57E0A5695B3C}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6565C9D7-7AF9-442D-98FF-0511CAF4172B}" name="NSCCITSWebDCourses" displayName="NSCCITSWebDCourses" ref="A1:B53" tableType="queryTable" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:B53" xr:uid="{F8C5946E-C848-4CEC-AF26-DD6D7F2DF38A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6565C9D7-7AF9-442D-98FF-0511CAF4172B}" name="NSCCITSWebDCourses" displayName="NSCCITSWebDCourses" ref="A1:B51" tableType="queryTable" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:B51" xr:uid="{F8C5946E-C848-4CEC-AF26-DD6D7F2DF38A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{61158880-33E3-4E6F-833B-2B9473C3FF06}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{5EC2F65D-5628-44D9-B395-2BBDD7C00074}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{61158880-33E3-4E6F-833B-2B9473C3FF06}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5EC2F65D-5628-44D9-B395-2BBDD7C00074}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FAAA48AE-C694-4BE9-A8F1-D926DE7BD070}" name="NSCCITProgCourses" displayName="NSCCITProgCourses" ref="A1:B53" tableType="queryTable" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:B53" xr:uid="{E36FD254-0DE7-4B77-A194-22B4DAF388CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FAAA48AE-C694-4BE9-A8F1-D926DE7BD070}" name="NSCCITProgCourses" displayName="NSCCITProgCourses" ref="A1:B51" tableType="queryTable" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A1:B51" xr:uid="{E36FD254-0DE7-4B77-A194-22B4DAF388CB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7F9796A6-27F6-4715-A2E4-00190A90D376}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CFD9A2C7-541A-402C-A953-BBED086D669B}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{7F9796A6-27F6-4715-A2E4-00190A90D376}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{CFD9A2C7-541A-402C-A953-BBED086D669B}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D08CCF6B-3026-43D5-9E17-B0B8AB84FEE6}" name="NSCCITGenCourses" displayName="NSCCITGenCourses" ref="A1:B59" tableType="queryTable" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:B59" xr:uid="{EF13D13D-2392-4923-B082-1C3AD5F0B2F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D08CCF6B-3026-43D5-9E17-B0B8AB84FEE6}" name="NSCCITGenCourses" displayName="NSCCITGenCourses" ref="A1:B57" tableType="queryTable" totalsRowShown="0" dataDxfId="12">
+  <autoFilter ref="A1:B57" xr:uid="{EF13D13D-2392-4923-B082-1C3AD5F0B2F2}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{782396D8-CCCB-4F47-B677-57DC726E486B}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{D992E8CD-8F28-4B6D-ABDB-65EF16AFD69E}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="10"/>
@@ -851,33 +851,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{592B029B-1E9A-43F1-9CD3-3390C3922B34}" name="NSCCITEmbeddedSysCourses" displayName="NSCCITEmbeddedSysCourses" ref="A1:B33" tableType="queryTable" totalsRowShown="0" dataDxfId="12">
-  <autoFilter ref="A1:B33" xr:uid="{591CE723-3670-4EDA-9E44-2BE57A81B062}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{592B029B-1E9A-43F1-9CD3-3390C3922B34}" name="NSCCITEmbeddedSysCourses" displayName="NSCCITEmbeddedSysCourses" ref="A1:B31" tableType="queryTable" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:B31" xr:uid="{591CE723-3670-4EDA-9E44-2BE57A81B062}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BE22E571-BE76-4995-BFDA-D3F472D553E0}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{B739D3FA-CAF6-430F-B306-0AA0B3F18798}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{BE22E571-BE76-4995-BFDA-D3F472D553E0}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B739D3FA-CAF6-430F-B306-0AA0B3F18798}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AFEFE05-65AD-4B84-A339-9E7F19D2204D}" name="NSCCITDbasAdminCourses" displayName="NSCCITDbasAdminCourses" ref="A1:B63" tableType="queryTable" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="A1:B63" xr:uid="{2B6FFAC4-0167-402F-B0B6-188D1ED122B6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AFEFE05-65AD-4B84-A339-9E7F19D2204D}" name="NSCCITDbasAdminCourses" displayName="NSCCITDbasAdminCourses" ref="A1:B61" tableType="queryTable" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:B61" xr:uid="{2B6FFAC4-0167-402F-B0B6-188D1ED122B6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{66542ED5-DB08-42A7-8D53-5E6C11E58AB0}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{1CB9AFF7-414D-4489-A99B-28F72216A21F}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{66542ED5-DB08-42A7-8D53-5E6C11E58AB0}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{1CB9AFF7-414D-4489-A99B-28F72216A21F}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B06D50F2-1D73-476B-AB1E-366D6537A15D}" name="NSCCITDataAnlsCourses" displayName="NSCCITDataAnlsCourses" ref="A1:B63" tableType="queryTable" totalsRowShown="0" dataDxfId="18">
-  <autoFilter ref="A1:B63" xr:uid="{8BA241DB-CE79-4317-B4DE-FD432884C0A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B06D50F2-1D73-476B-AB1E-366D6537A15D}" name="NSCCITDataAnlsCourses" displayName="NSCCITDataAnlsCourses" ref="A1:B61" tableType="queryTable" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:B61" xr:uid="{8BA241DB-CE79-4317-B4DE-FD432884C0A9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{710A6AE5-AA25-4FED-8FE1-1A8D1895A5AE}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{6AAF0112-2A51-4BF7-A4E7-7496665A2D27}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{710A6AE5-AA25-4FED-8FE1-1A8D1895A5AE}" uniqueName="1" name="Course Title" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{6AAF0112-2A51-4BF7-A4E7-7496665A2D27}" uniqueName="2" name="Course Description" queryTableFieldId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26345A3-132B-4BC9-B46C-283E0948A133}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,6 +1166,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
@@ -1174,12 +1182,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1190,12 +1198,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1208,10 +1216,10 @@
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1222,12 +1230,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1238,12 +1246,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1254,12 +1262,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1270,12 +1278,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1286,12 +1294,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1302,12 +1310,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1318,12 +1326,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1334,12 +1342,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1350,12 +1358,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1366,12 +1374,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1382,12 +1390,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1398,12 +1406,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1414,12 +1422,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>163</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1430,12 +1438,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1446,12 +1454,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1462,12 +1470,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1478,12 +1486,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1494,12 +1502,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1510,12 +1518,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1526,12 +1534,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1542,12 +1550,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>119</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1558,12 +1566,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>173</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1574,12 +1582,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1592,10 +1600,10 @@
     </row>
     <row r="56" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1608,10 +1616,10 @@
     </row>
     <row r="58" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1619,22 +1627,6 @@
         <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1648,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A6FC6A-E864-4A5A-B394-9EB1DB8A4704}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,6 +1660,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
@@ -1676,12 +1676,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1692,12 +1692,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1708,12 +1708,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1726,10 +1726,10 @@
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1740,12 +1740,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1756,12 +1756,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1772,12 +1772,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1788,12 +1788,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1804,12 +1804,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1822,10 +1822,10 @@
     </row>
     <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1836,12 +1836,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1852,12 +1852,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1870,10 +1870,10 @@
     </row>
     <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1884,12 +1884,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1900,12 +1900,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1916,12 +1916,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1932,12 +1932,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1950,10 +1950,10 @@
     </row>
     <row r="38" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1966,10 +1966,10 @@
     </row>
     <row r="40" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1982,10 +1982,10 @@
     </row>
     <row r="42" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1996,12 +1996,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2012,12 +2012,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2028,12 +2028,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2044,12 +2044,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2057,22 +2057,6 @@
         <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2086,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FDB410-1115-4FFD-8094-F43DEF129E98}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,6 +2090,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
@@ -2114,12 +2106,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2130,12 +2122,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2146,12 +2138,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2164,10 +2156,10 @@
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2178,12 +2170,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2194,12 +2186,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2210,12 +2202,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2226,12 +2218,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2242,12 +2234,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2258,12 +2250,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2274,12 +2266,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2290,12 +2282,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2306,12 +2298,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2322,12 +2314,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2338,12 +2330,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2354,12 +2346,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2372,10 +2364,10 @@
     </row>
     <row r="36" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2388,10 +2380,10 @@
     </row>
     <row r="38" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2402,12 +2394,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2420,10 +2412,10 @@
     </row>
     <row r="42" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2434,12 +2426,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2452,10 +2444,10 @@
     </row>
     <row r="46" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2468,10 +2460,10 @@
     </row>
     <row r="48" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2482,12 +2474,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2495,22 +2487,6 @@
         <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2524,10 +2500,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BAE8EF-B84C-4639-AA07-6AB9A99E8FA9}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2544,6 +2520,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
@@ -2552,12 +2536,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2568,12 +2552,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2584,12 +2568,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2602,10 +2586,10 @@
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2618,10 +2602,10 @@
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2632,12 +2616,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2648,12 +2632,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2664,12 +2648,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2680,12 +2664,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2696,12 +2680,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2712,12 +2696,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2728,12 +2712,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2744,12 +2728,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2762,10 +2746,10 @@
     </row>
     <row r="30" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2776,12 +2760,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2792,12 +2776,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2808,12 +2792,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2824,12 +2808,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2840,12 +2824,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2856,12 +2840,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2872,12 +2856,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2888,12 +2872,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2904,12 +2888,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2920,12 +2904,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2938,10 +2922,10 @@
     </row>
     <row r="52" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2952,12 +2936,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -2968,12 +2952,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2981,22 +2965,6 @@
         <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3010,10 +2978,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E851DFEB-FF43-44C4-8EB6-EAB5FE2C70EE}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,8 +2998,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3041,12 +3014,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3057,12 +3030,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3075,10 +3048,10 @@
     </row>
     <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3089,12 +3062,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3105,12 +3078,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3121,12 +3094,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3137,12 +3110,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3155,10 +3128,10 @@
     </row>
     <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3169,12 +3142,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3185,12 +3158,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3203,10 +3176,10 @@
     </row>
     <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3217,12 +3190,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -3235,10 +3208,10 @@
     </row>
     <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -3251,10 +3224,10 @@
     </row>
     <row r="30" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3262,22 +3235,6 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3291,10 +3248,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6D64E0-F015-4B14-8432-3AA080929475}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3311,6 +3268,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
@@ -3319,12 +3284,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3335,12 +3300,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3353,10 +3318,10 @@
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3367,12 +3332,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3383,12 +3348,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3399,12 +3364,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3415,12 +3380,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3433,10 +3398,10 @@
     </row>
     <row r="18" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3447,12 +3412,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3465,10 +3430,10 @@
     </row>
     <row r="22" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3479,12 +3444,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3495,12 +3460,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -3511,12 +3476,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -3529,10 +3494,10 @@
     </row>
     <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3543,12 +3508,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3559,12 +3524,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3591,12 +3556,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3607,12 +3572,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3623,12 +3588,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3639,12 +3604,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -3655,12 +3620,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -3671,12 +3636,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -3687,12 +3652,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -3703,12 +3668,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -3719,12 +3684,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -3737,10 +3702,10 @@
     </row>
     <row r="56" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -3751,12 +3716,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -3767,12 +3732,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -3780,22 +3745,6 @@
         <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3809,7 +3758,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE2D4B9-CF32-4A9A-A197-2A25BF064D7D}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -3829,20 +3778,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3853,12 +3810,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3869,12 +3826,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3887,10 +3844,10 @@
     </row>
     <row r="10" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3901,12 +3858,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3917,12 +3874,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3933,12 +3890,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3949,12 +3906,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3965,12 +3922,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3981,12 +3938,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3997,12 +3954,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4013,12 +3970,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4029,12 +3986,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -4045,12 +4002,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -4063,10 +4020,10 @@
     </row>
     <row r="32" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4077,12 +4034,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -4095,10 +4052,10 @@
     </row>
     <row r="36" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -4109,12 +4066,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -4125,12 +4082,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -4141,12 +4098,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -4157,12 +4114,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -4173,12 +4130,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -4189,12 +4146,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -4205,12 +4162,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -4221,12 +4178,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -4237,12 +4194,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -4253,12 +4210,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -4271,10 +4228,10 @@
     </row>
     <row r="58" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -4285,12 +4242,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -4298,22 +4255,6 @@
         <v>2</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>